<commit_message>
added conclusions to benchmarking summary
</commit_message>
<xml_diff>
--- a/MASH-dev/AlecGeorgoff/Benchmarking/BM_outline/benchmarking_outline.xlsx
+++ b/MASH-dev/AlecGeorgoff/Benchmarking/BM_outline/benchmarking_outline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11270" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17030" windowHeight="4840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="20">
   <si>
     <t>n_humans</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>memory (kB)</t>
+  </si>
+  <si>
+    <t>runtime (min)</t>
+  </si>
+  <si>
+    <t>runtime (hr)</t>
+  </si>
+  <si>
+    <t>memory (MB)</t>
   </si>
 </sst>
 </file>
@@ -193,7 +202,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,6 +288,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1906,10 +1918,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1921,9 +1933,11 @@
     <col min="5" max="5" width="4.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1942,8 +1956,14 @@
       <c r="G1" s="23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
@@ -1965,8 +1985,16 @@
       <c r="G2" s="17">
         <v>95632</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="32">
+        <f>F2/60</f>
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="I2" s="32">
+        <f>G2/1000</f>
+        <v>95.632000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="25"/>
       <c r="B3" s="1">
         <v>500</v>
@@ -1986,8 +2014,16 @@
       <c r="G3" s="19">
         <v>98396</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="33">
+        <f t="shared" ref="H3:H6" si="0">F3/60</f>
+        <v>1.4404000000000001</v>
+      </c>
+      <c r="I3" s="33">
+        <f t="shared" ref="I3:I6" si="1">G3/1000</f>
+        <v>98.396000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="25"/>
       <c r="B4" s="1">
         <v>500</v>
@@ -2007,8 +2043,16 @@
       <c r="G4" s="19">
         <v>102200</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="33">
+        <f t="shared" si="0"/>
+        <v>4.5877499999999998</v>
+      </c>
+      <c r="I4" s="33">
+        <f t="shared" si="1"/>
+        <v>102.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="25"/>
       <c r="B5" s="1">
         <v>500</v>
@@ -2028,8 +2072,16 @@
       <c r="G5" s="19">
         <v>104048</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="33">
+        <f t="shared" si="0"/>
+        <v>13.5678</v>
+      </c>
+      <c r="I5" s="33">
+        <f t="shared" si="1"/>
+        <v>104.048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="26"/>
       <c r="B6" s="2">
         <v>500</v>
@@ -2049,8 +2101,16 @@
       <c r="G6" s="2">
         <v>107180</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="31">
+        <f t="shared" si="0"/>
+        <v>27.248316666666664</v>
+      </c>
+      <c r="I6" s="31">
+        <f t="shared" si="1"/>
+        <v>107.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
@@ -2069,8 +2129,14 @@
       <c r="G8" s="23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>4</v>
       </c>
@@ -2092,8 +2158,16 @@
       <c r="G9" s="17">
         <v>318336</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="32">
+        <f>F9/3600</f>
+        <v>5.284888888888889E-2</v>
+      </c>
+      <c r="I9" s="32">
+        <f>G9/1000</f>
+        <v>318.33600000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="25"/>
       <c r="B10" s="1">
         <v>5000</v>
@@ -2113,8 +2187,16 @@
       <c r="G10" s="19">
         <v>308072</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="33">
+        <f t="shared" ref="H10:H13" si="2">F10/3600</f>
+        <v>0.10323666666666666</v>
+      </c>
+      <c r="I10" s="33">
+        <f t="shared" ref="I10:I13" si="3">G10/1000</f>
+        <v>308.072</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="25"/>
       <c r="B11" s="1">
         <v>5000</v>
@@ -2134,8 +2216,16 @@
       <c r="G11" s="19">
         <v>308848</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="33">
+        <f t="shared" si="2"/>
+        <v>0.3898833333333333</v>
+      </c>
+      <c r="I11" s="33">
+        <f t="shared" si="3"/>
+        <v>308.84800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="25"/>
       <c r="B12" s="1">
         <v>5000</v>
@@ -2155,8 +2245,16 @@
       <c r="G12" s="19">
         <v>311320</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="33">
+        <f t="shared" si="2"/>
+        <v>1.1927158333333334</v>
+      </c>
+      <c r="I12" s="33">
+        <f t="shared" si="3"/>
+        <v>311.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="26"/>
       <c r="B13" s="2">
         <v>5000</v>
@@ -2176,8 +2274,16 @@
       <c r="G13" s="2">
         <v>316616</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="31">
+        <f t="shared" si="2"/>
+        <v>3.5063894444444443</v>
+      </c>
+      <c r="I13" s="31">
+        <f t="shared" si="3"/>
+        <v>316.61599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
@@ -2196,8 +2302,14 @@
       <c r="G15" s="23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>5</v>
       </c>
@@ -2219,8 +2331,16 @@
       <c r="G16" s="17">
         <v>2122120</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" s="32">
+        <f>F16/3600</f>
+        <v>2.1766119444444443</v>
+      </c>
+      <c r="I16" s="32">
+        <f>G16/1000</f>
+        <v>2122.12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="25"/>
       <c r="B17" s="3">
         <v>50000</v>
@@ -2240,8 +2360,16 @@
       <c r="G17" s="19">
         <v>2135744</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="33">
+        <f t="shared" ref="H17:H19" si="4">F17/3600</f>
+        <v>2.5108058333333334</v>
+      </c>
+      <c r="I17" s="33">
+        <f t="shared" ref="I17:I19" si="5">G17/1000</f>
+        <v>2135.7440000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="25"/>
       <c r="B18" s="3">
         <v>50000</v>
@@ -2261,8 +2389,16 @@
       <c r="G18" s="19">
         <v>2222924</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" s="33">
+        <f t="shared" si="4"/>
+        <v>3.8828608333333334</v>
+      </c>
+      <c r="I18" s="33">
+        <f t="shared" si="5"/>
+        <v>2222.924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="26"/>
       <c r="B19" s="4">
         <v>50000</v>
@@ -2282,8 +2418,16 @@
       <c r="G19" s="2">
         <v>6633904</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" s="31">
+        <f t="shared" si="4"/>
+        <v>6.8561755555555557</v>
+      </c>
+      <c r="I19" s="31">
+        <f t="shared" si="5"/>
+        <v>6633.9040000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>0</v>
       </c>
@@ -2302,8 +2446,14 @@
       <c r="G21" s="23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>6</v>
       </c>
@@ -2325,8 +2475,16 @@
       <c r="G22" s="17">
         <v>85768</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" s="32">
+        <f>F22/60</f>
+        <v>0.51611666666666667</v>
+      </c>
+      <c r="I22" s="32">
+        <f>G22/1000</f>
+        <v>85.768000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="25"/>
       <c r="B23" s="3">
         <v>300</v>
@@ -2346,8 +2504,16 @@
       <c r="G23" s="19">
         <v>103112</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" s="33">
+        <f t="shared" ref="H23:H27" si="6">F23/60</f>
+        <v>0.49756666666666666</v>
+      </c>
+      <c r="I23" s="33">
+        <f t="shared" ref="I23:I27" si="7">G23/1000</f>
+        <v>103.11199999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="25"/>
       <c r="B24" s="3">
         <v>1000</v>
@@ -2367,8 +2533,16 @@
       <c r="G24" s="19">
         <v>193276</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" s="33">
+        <f t="shared" si="6"/>
+        <v>3.6243833333333333</v>
+      </c>
+      <c r="I24" s="33">
+        <f t="shared" si="7"/>
+        <v>193.27600000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="25"/>
       <c r="B25" s="3">
         <v>3000</v>
@@ -2388,8 +2562,16 @@
       <c r="G25" s="19">
         <v>298288</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" s="33">
+        <f t="shared" si="6"/>
+        <v>14.449149999999999</v>
+      </c>
+      <c r="I25" s="33">
+        <f t="shared" si="7"/>
+        <v>298.28800000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="25"/>
       <c r="B26" s="3">
         <v>10000</v>
@@ -2409,8 +2591,16 @@
       <c r="G26" s="19">
         <v>575324</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" s="33">
+        <f t="shared" si="6"/>
+        <v>38.631216666666667</v>
+      </c>
+      <c r="I26" s="33">
+        <f t="shared" si="7"/>
+        <v>575.32399999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
       <c r="B27" s="4">
         <v>30000</v>
@@ -2430,8 +2620,16 @@
       <c r="G27" s="2">
         <v>2010632</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" s="31">
+        <f t="shared" si="6"/>
+        <v>175.94329999999999</v>
+      </c>
+      <c r="I27" s="31">
+        <f t="shared" si="7"/>
+        <v>2010.6320000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="10"/>
       <c r="B29" s="5" t="s">
         <v>0</v>
@@ -2451,8 +2649,14 @@
       <c r="G29" s="23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="24" t="s">
         <v>13</v>
       </c>
@@ -2474,8 +2678,16 @@
       <c r="G30" s="17">
         <v>133636</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" s="32">
+        <f>F30/3600</f>
+        <v>5.035916666666667E-2</v>
+      </c>
+      <c r="I30" s="32">
+        <f>G30/1000</f>
+        <v>133.636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="25"/>
       <c r="B31" s="3">
         <v>3000</v>
@@ -2495,8 +2707,16 @@
       <c r="G31" s="19">
         <v>214384</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" s="33">
+        <f t="shared" ref="H31:H36" si="8">F31/3600</f>
+        <v>0.17094027777777779</v>
+      </c>
+      <c r="I31" s="33">
+        <f t="shared" ref="I31:I36" si="9">G31/1000</f>
+        <v>214.38399999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="25"/>
       <c r="B32" s="3">
         <v>10000</v>
@@ -2516,8 +2736,16 @@
       <c r="G32" s="19">
         <v>519560</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" s="33">
+        <f t="shared" si="8"/>
+        <v>0.39114305555555556</v>
+      </c>
+      <c r="I32" s="33">
+        <f t="shared" si="9"/>
+        <v>519.55999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="25"/>
       <c r="B33" s="3">
         <v>30000</v>
@@ -2537,8 +2765,16 @@
       <c r="G33" s="19">
         <v>1238356</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" s="33">
+        <f t="shared" si="8"/>
+        <v>1.1376161111111112</v>
+      </c>
+      <c r="I33" s="33">
+        <f t="shared" si="9"/>
+        <v>1238.356</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="25"/>
       <c r="B34" s="3">
         <v>100000</v>
@@ -2558,8 +2794,16 @@
       <c r="G34" s="19">
         <v>4364848</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" s="33">
+        <f t="shared" si="8"/>
+        <v>5.1681833333333334</v>
+      </c>
+      <c r="I34" s="33">
+        <f t="shared" si="9"/>
+        <v>4364.848</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="25"/>
       <c r="B35" s="3">
         <v>200000</v>
@@ -2579,8 +2823,16 @@
       <c r="G35" s="19">
         <v>7522608</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" s="33">
+        <f t="shared" si="8"/>
+        <v>15.892144166666666</v>
+      </c>
+      <c r="I35" s="33">
+        <f t="shared" si="9"/>
+        <v>7522.6080000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="26"/>
       <c r="B36" s="2">
         <v>300000</v>
@@ -2600,8 +2852,16 @@
       <c r="G36" s="2">
         <v>12940308</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" s="31">
+        <f t="shared" si="8"/>
+        <v>36.359323611111108</v>
+      </c>
+      <c r="I36" s="31">
+        <f t="shared" si="9"/>
+        <v>12940.308000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B38" s="22" t="s">
         <v>0</v>
       </c>
@@ -2620,8 +2880,14 @@
       <c r="G38" s="23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
         <v>14</v>
       </c>
@@ -2643,8 +2909,16 @@
       <c r="G39" s="17">
         <v>143756</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" s="32">
+        <f>F39/3600</f>
+        <v>2.4561666666666666E-2</v>
+      </c>
+      <c r="I39" s="32">
+        <f>G39/1000</f>
+        <v>143.756</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="25"/>
       <c r="B40" s="3">
         <v>3000</v>
@@ -2664,8 +2938,16 @@
       <c r="G40" s="19">
         <v>221852</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" s="33">
+        <f t="shared" ref="H40:H45" si="10">F40/3600</f>
+        <v>7.6030833333333339E-2</v>
+      </c>
+      <c r="I40" s="33">
+        <f t="shared" ref="I40:I45" si="11">G40/1000</f>
+        <v>221.852</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="25"/>
       <c r="B41" s="3">
         <v>10000</v>
@@ -2685,8 +2967,16 @@
       <c r="G41" s="19">
         <v>526180</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" s="33">
+        <f t="shared" si="10"/>
+        <v>0.29037000000000002</v>
+      </c>
+      <c r="I41" s="33">
+        <f t="shared" si="11"/>
+        <v>526.17999999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="25"/>
       <c r="B42" s="3">
         <v>30000</v>
@@ -2706,8 +2996,16 @@
       <c r="G42" s="19">
         <v>1243984</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" s="33">
+        <f t="shared" si="10"/>
+        <v>0.97648888888888896</v>
+      </c>
+      <c r="I42" s="33">
+        <f t="shared" si="11"/>
+        <v>1243.9839999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="25"/>
       <c r="B43" s="3">
         <v>100000</v>
@@ -2727,8 +3025,16 @@
       <c r="G43" s="19">
         <v>4372520</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" s="33">
+        <f t="shared" si="10"/>
+        <v>4.9546161111111111</v>
+      </c>
+      <c r="I43" s="33">
+        <f t="shared" si="11"/>
+        <v>4372.5200000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="25"/>
       <c r="B44" s="3">
         <v>200000</v>
@@ -2748,8 +3054,16 @@
       <c r="G44" s="19">
         <v>7529200</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" s="33">
+        <f t="shared" si="10"/>
+        <v>13.920281666666668</v>
+      </c>
+      <c r="I44" s="33">
+        <f t="shared" si="11"/>
+        <v>7529.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="26"/>
       <c r="B45" s="2">
         <v>300000</v>
@@ -2769,15 +3083,23 @@
       <c r="G45" s="2">
         <v>12968196</v>
       </c>
+      <c r="H45" s="31">
+        <f t="shared" si="10"/>
+        <v>30.177984166666668</v>
+      </c>
+      <c r="I45" s="31">
+        <f t="shared" si="11"/>
+        <v>12968.196</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A39:A45"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A22:A27"/>
     <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A39:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>